<commit_message>
Add another PairedData test
refactoring, including consolidate some error messages
</commit_message>
<xml_diff>
--- a/test-files/simple-paired-data.xlsx
+++ b/test-files/simple-paired-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\DSSExcel\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F683E4DC-DE71-4B0C-BA90-9A3D68108C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43CB9F-A0B5-460F-A3A7-EFEB2D004CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34785" yWindow="1605" windowWidth="18750" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31245" yWindow="840" windowWidth="18750" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Labels</t>
   </si>
@@ -40,13 +40,16 @@
     <t>Type</t>
   </si>
   <si>
-    <t>UNT</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
     <t>/A/B/Elevation-Flow////</t>
+  </si>
+  <si>
+    <t>UNT1</t>
+  </si>
+  <si>
+    <t>UNT2</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,10 +421,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,10 +454,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>